<commit_message>
added template for pbSettings - pb
</commit_message>
<xml_diff>
--- a/Templates/pbSettingsTemplate.xlsx
+++ b/Templates/pbSettingsTemplate.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrower/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrower/projects/just-VBA/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59904F9C-FD5A-C841-ADCA-D837FE2D459A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335B9D4E-730A-074C-ADEC-2AD3D8913783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10920" yWindow="5880" windowWidth="27640" windowHeight="16940" xr2:uid="{81D820F5-EA99-EA42-B651-814247F84A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="WKBKSettings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -189,41 +189,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF1F4E78"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD7DCE4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="3" tint="0.39994506668294322"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -310,16 +275,51 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color rgb="FF1F4E78"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color theme="5" tint="-0.24994659260841701"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF1F4E78"/>
-        </top>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF1F4E78"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD7DCE4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="3" tint="0.39994506668294322"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -336,13 +336,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4ADA89B6-E0F7-634D-A55F-E68AC3BA359A}" name="tbl_pbSettings" displayName="tbl_pbSettings" ref="A6:D7" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4ADA89B6-E0F7-634D-A55F-E68AC3BA359A}" name="tbl_pbSettings" displayName="tbl_pbSettings" ref="A6:D7" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A6:D7" xr:uid="{4ADA89B6-E0F7-634D-A55F-E68AC3BA359A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ADB36D7D-BB79-C249-932A-7C74295A56EB}" name="SettingKey" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D96B8EBB-B93D-704B-8B7B-2A525E21A1C7}" name="SettingValue" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{1A9DA52E-ABAD-4A40-AE31-B1967300979D}" name="SettingType" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{4527E3A3-123B-644B-A563-FEBAED965D02}" name="Updated" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{ADB36D7D-BB79-C249-932A-7C74295A56EB}" name="SettingKey" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D96B8EBB-B93D-704B-8B7B-2A525E21A1C7}" name="SettingValue" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1A9DA52E-ABAD-4A40-AE31-B1967300979D}" name="SettingType" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4527E3A3-123B-644B-A563-FEBAED965D02}" name="Updated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -645,7 +645,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0B404D-FAA8-E346-85DA-E188CA92952A}">
-  <sheetPr codeName="pbSettingsWS"/>
+  <sheetPr codeName="pbSTGWS"/>
   <dimension ref="A6:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
created pbSettings.cls - stand-alone complete settings management for your VBA workbook - pb
</commit_message>
<xml_diff>
--- a/Templates/pbSettingsTemplate.xlsx
+++ b/Templates/pbSettingsTemplate.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr codeName="justVBASettingTemplate" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrower/projects/just-VBA/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335B9D4E-730A-074C-ADEC-2AD3D8913783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722F1B83-C04E-2044-9A94-598B7C33080E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10920" yWindow="5880" windowWidth="27640" windowHeight="16940" xr2:uid="{81D820F5-EA99-EA42-B651-814247F84A6F}"/>
   </bookViews>
@@ -649,7 +649,7 @@
   <dimension ref="A6:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>